<commit_message>
Added filament tip analysis
</commit_message>
<xml_diff>
--- a/Linienlaser/_Messbedingungen.xlsx
+++ b/Linienlaser/_Messbedingungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECTS\Dissertation\FilamentCounting\GitHub\filament-counting\Linienlaser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AF1A2D-2EDA-4320-A085-406A1871A833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB6AFEE-4F79-4CCB-A6E5-4751F17FCFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="348" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9972" yWindow="2844" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Umdrehungen</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>0.7</t>
+  </si>
+  <si>
+    <t>BU6981_2U_L.csv</t>
+  </si>
+  <si>
+    <t>906 22705</t>
+  </si>
+  <si>
+    <t>0.35</t>
   </si>
 </sst>
 </file>
@@ -787,10 +796,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BC58C6-5D54-4B3A-9EBB-1592C6FAECAE}">
-  <dimension ref="B2:H4"/>
+  <dimension ref="B2:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,7 +807,7 @@
     <col min="1" max="1" width="3.21875" style="8" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.21875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
@@ -874,6 +883,29 @@
         <v>28</v>
       </c>
     </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="8">
+        <v>50</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="8">
+        <v>50</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>